<commit_message>
[FIX] Fix a bug in deducting loans
</commit_message>
<xml_diff>
--- a/erpnext-notes/NEXTERP-NOTES.xlsx
+++ b/erpnext-notes/NEXTERP-NOTES.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="14"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Functional" sheetId="1" state="visible" r:id="rId2"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="376">
   <si>
     <t xml:space="preserve">Supplier can be an individual or an organization and has multiple Contacts and Addresses</t>
   </si>
@@ -94,6 +94,12 @@
     <t xml:space="preserve">book of accounts == chart of accounts?????</t>
   </si>
   <si>
+    <t xml:space="preserve">Basics of accounting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://frappebooks.com/docs</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bench is a command line utility to install, manage multiple sites and manage the ERPNext application on a Unix-based system</t>
   </si>
   <si>
@@ -1141,32 +1147,8 @@
     <t xml:space="preserve">Adding app to a site</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">bench get-app </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">https://github.com/org/app_name</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> + 
+    <t xml:space="preserve">bench get-app https://github.com/org/app_name + 
 bench --site site_name install-app app_name</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">To set the self.name property in the method</t>
@@ -1179,6 +1161,12 @@
   </si>
   <si>
     <t xml:space="preserve">https://frappeframework.com/docs/user/en/guides/app-development/exporting-customizations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Insert A Document Via Api</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://frappeframework.com/docs/user/en/guides/app-development/insert-a-document-via-api</t>
   </si>
   <si>
     <t xml:space="preserve">Bench is the all-in-one tool to manage all things Frappe</t>
@@ -2081,6 +2069,12 @@
     <t xml:space="preserve">To create a module icon for a Page, List or Module, you will have to edit the config/desktop.py file in your app or add a.py file with the module name</t>
   </si>
   <si>
+    <t xml:space="preserve">Overriding Link Query By Custom Script</t>
+  </si>
+  <si>
+    <t xml:space="preserve">override the standard link query by using set_query for Adding Filters or Calling a Different Method to Generate Results </t>
+  </si>
+  <si>
     <t xml:space="preserve">setting date format</t>
   </si>
   <si>
@@ -2147,12 +2141,18 @@
     <t xml:space="preserve">Common utilities</t>
   </si>
   <si>
-    <t xml:space="preserve">https://frappeframework.com/docs/user/en/api/dialog#dialog-api</t>
+    <t xml:space="preserve">https://frappeframework.com/docs/user/en/api/dialog#dialog-api </t>
   </si>
   <si>
     <t xml:space="preserve">Dialogs</t>
   </si>
   <si>
+    <t xml:space="preserve">https://frappeframework.com/docs/user/en/guides/app-development/dialogs-types</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dialogs Types</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://www.frappeframework.com/docs//user/en/bench/resources/bench-commands-cheatsheet</t>
   </si>
   <si>
@@ -2202,26 +2202,16 @@
     <t xml:space="preserve">https://frappeframework.com/docs/user/en/guides/app-development/adding-module-icons-on-desktop</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">https://frappeframework.com/docs/user/en/guides/app-development/custom-module</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">-icon</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">adding custom module icon</t>
+    <t xml:space="preserve">https://frappeframework.com/docs/user/en/guides/app-development/custom-module-icon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adding custom module icon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://frappeframework.com/docs/user/en/guides/app-development/overriding-link-query-by-custom-script</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Overriding Link Query By Custom Script ( 2 add domain 4exm)</t>
   </si>
   <si>
     <t xml:space="preserve">Frappe Controls</t>
@@ -2236,6 +2226,15 @@
     <t xml:space="preserve">What is next server_action and  client_side</t>
   </si>
   <si>
+    <t xml:space="preserve">patch in the patches.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">how to add x2many in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">buttons groups on erpnext</t>
+  </si>
+  <si>
     <t xml:space="preserve">Issue</t>
   </si>
   <si>
@@ -2267,6 +2266,13 @@
   </si>
   <si>
     <t xml:space="preserve">https://frappeframework.com/docs/user/en/guides/app-development/how-to-create-custom-fields-during-app-installation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extending Documents: Each model can be extended by adding events in the controller class
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://frappe.io/frappejs/docs/models/document.md</t>
   </si>
 </sst>
 </file>
@@ -2381,13 +2387,13 @@
       <family val="2"/>
     </font>
     <font>
-      <b val="true"/>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
+      <b val="true"/>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
@@ -2541,6 +2547,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFDB7093"/>
+        <bgColor rgb="FFFF69B4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF6B8E23"/>
         <bgColor rgb="FF808000"/>
       </patternFill>
@@ -2591,12 +2603,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF69B4"/>
         <bgColor rgb="FFDB7093"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDB7093"/>
-        <bgColor rgb="FFFF69B4"/>
       </patternFill>
     </fill>
     <fill>
@@ -2760,7 +2766,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="68">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2785,7 +2791,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="13" fillId="14" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2801,31 +2815,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="14" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="16" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="15" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="16" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="17" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="16" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="17" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2833,19 +2843,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="17" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="18" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="17" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="18" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="18" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="19" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="18" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="23" fillId="19" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2853,26 +2863,18 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="19" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="20" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="20" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="21" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="20" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="21" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="21" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="22" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2881,11 +2883,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="23" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="23" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="23" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="23" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="14" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2985,11 +2995,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="16" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="16" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="25" fillId="17" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="17" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3001,7 +3011,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="33" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3126,7 +3136,7 @@
   <dimension ref="A2:A7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3177,10 +3187,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3190,26 +3200,26 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="68.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="8" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="3" s="35" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="35" t="s">
-        <v>296</v>
+      <c r="A1" s="10" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="3" s="36" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="36" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="s">
-        <v>298</v>
+      <c r="A5" s="9" t="s">
+        <v>302</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>2</v>
@@ -3217,7 +3227,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>3</v>
@@ -3225,7 +3235,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>4</v>
@@ -3233,7 +3243,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>5</v>
@@ -3241,17 +3251,17 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8" t="s">
-        <v>303</v>
+      <c r="A10" s="10" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>6</v>
@@ -3259,40 +3269,50 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="10" t="s">
-        <v>306</v>
+      <c r="A15" s="12" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="47" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="18" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="7" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="21" s="44" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="43" t="s">
-        <v>310</v>
+      <c r="A17" s="48" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="18" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="9" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="21" s="45" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="44" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>311</v>
+        <v>315</v>
+      </c>
+    </row>
+    <row r="24" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="9" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>317</v>
       </c>
     </row>
   </sheetData>
@@ -3325,10 +3345,10 @@
   <sheetData>
     <row r="2" customFormat="false" ht="13.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>312</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>313</v>
+        <v>318</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>319</v>
       </c>
     </row>
   </sheetData>
@@ -3347,220 +3367,244 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="89.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="46.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="70.76"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="16" t="s">
-        <v>314</v>
+      <c r="A1" s="7" t="s">
+        <v>320</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>315</v>
+        <v>321</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="16" t="s">
-        <v>316</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>317</v>
+      <c r="A2" s="7" t="s">
+        <v>322</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>318</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>319</v>
+        <v>324</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="16" t="s">
-        <v>320</v>
+      <c r="A4" s="7" t="s">
+        <v>326</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>321</v>
+        <v>327</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="16" t="s">
-        <v>322</v>
+      <c r="A5" s="7" t="s">
+        <v>328</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>323</v>
+        <v>329</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>324</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>325</v>
+        <v>330</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="9"/>
+      <c r="A7" s="11"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="16" t="s">
-        <v>150</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="9" s="62" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="60" t="s">
-        <v>158</v>
-      </c>
-      <c r="B9" s="61" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="10" s="62" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="60" t="s">
-        <v>326</v>
-      </c>
-      <c r="B10" s="61" t="s">
-        <v>244</v>
+      <c r="A8" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="9" s="63" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="61" t="s">
+        <v>160</v>
+      </c>
+      <c r="B9" s="62" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="10" s="63" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="61" t="s">
+        <v>332</v>
+      </c>
+      <c r="B10" s="62" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="16" t="s">
-        <v>160</v>
+      <c r="A11" s="7" t="s">
+        <v>162</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>327</v>
+        <v>333</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="16" t="s">
-        <v>133</v>
+      <c r="A12" s="7" t="s">
+        <v>135</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>328</v>
+        <v>334</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="16" t="s">
-        <v>135</v>
+      <c r="A13" s="7" t="s">
+        <v>137</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="16" t="s">
-        <v>329</v>
+      <c r="A14" s="7" t="s">
+        <v>335</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>330</v>
+        <v>336</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="16" t="s">
-        <v>169</v>
+      <c r="A15" s="7" t="s">
+        <v>171</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>331</v>
+        <v>337</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="16" t="s">
-        <v>169</v>
+      <c r="A16" s="7" t="s">
+        <v>171</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="16" t="s">
-        <v>171</v>
+      <c r="A17" s="7" t="s">
+        <v>173</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="16" t="s">
-        <v>332</v>
+      <c r="A18" s="7" t="s">
+        <v>338</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>333</v>
+        <v>339</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="16" t="s">
-        <v>334</v>
+      <c r="A19" s="7" t="s">
+        <v>340</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>335</v>
+        <v>341</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="10" t="s">
-        <v>336</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>337</v>
+      <c r="A20" s="7" t="s">
+        <v>342</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>343</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="16" t="s">
-        <v>338</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>339</v>
+      <c r="A21" s="12" t="s">
+        <v>344</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>345</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="16" t="s">
-        <v>340</v>
+      <c r="A22" s="7" t="s">
+        <v>346</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>341</v>
+        <v>347</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="16" t="s">
-        <v>181</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="16" t="s">
-        <v>343</v>
-      </c>
-      <c r="B24" s="0" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="16" t="s">
-        <v>344</v>
+      <c r="A23" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="7" t="s">
+        <v>351</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>345</v>
+        <v>314</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="16" t="s">
-        <v>187</v>
+      <c r="A26" s="7" t="s">
+        <v>352</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>186</v>
+        <v>353</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="7" t="s">
+        <v>354</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>355</v>
       </c>
     </row>
   </sheetData>
@@ -3581,12 +3625,15 @@
     <hyperlink ref="A17" r:id="rId14" display="https://frappeframework.com/docs/user/en/api/server-calls"/>
     <hyperlink ref="A18" r:id="rId15" display="https://frappeframework.com/docs/user/en/api/js-utils"/>
     <hyperlink ref="A19" r:id="rId16" location="dialog-api" display="https://frappeframework.com/docs/user/en/api/dialog#dialog-api"/>
-    <hyperlink ref="A20" r:id="rId17" display="https://www.frappeframework.com/docs//user/en/bench/resources/bench-commands-cheatsheet"/>
-    <hyperlink ref="A21" r:id="rId18" display="https://frappeframework.com/docs/user/en/tutorial/task-runner"/>
-    <hyperlink ref="A23" r:id="rId19" display="https://frappeframework.com/docs/user/en/guides/desk/formatter_for_link_fields"/>
-    <hyperlink ref="A24" r:id="rId20" display="https://frappeframework.com/docs/user/en/guides/app-development/adding-module-icons-on-desktop"/>
-    <hyperlink ref="A25" r:id="rId21" display="https://frappeframework.com/docs/user/en/guides/app-development/custom-module"/>
-    <hyperlink ref="A26" r:id="rId22" display="https://frappeframework.com/docs/user/en/guides/app-development/exporting-customizations"/>
+    <hyperlink ref="A20" r:id="rId17" display="https://frappeframework.com/docs/user/en/guides/app-development/dialogs-types"/>
+    <hyperlink ref="A21" r:id="rId18" display="https://www.frappeframework.com/docs//user/en/bench/resources/bench-commands-cheatsheet"/>
+    <hyperlink ref="A22" r:id="rId19" display="https://frappeframework.com/docs/user/en/tutorial/task-runner"/>
+    <hyperlink ref="A24" r:id="rId20" display="https://frappeframework.com/docs/user/en/guides/desk/formatter_for_link_fields"/>
+    <hyperlink ref="A25" r:id="rId21" display="https://frappeframework.com/docs/user/en/guides/app-development/adding-module-icons-on-desktop"/>
+    <hyperlink ref="A26" r:id="rId22" display="https://frappeframework.com/docs/user/en/guides/app-development/custom-module-icon"/>
+    <hyperlink ref="A27" r:id="rId23" display="https://frappeframework.com/docs/user/en/guides/app-development/exporting-customizations"/>
+    <hyperlink ref="A28" r:id="rId24" display="https://frappeframework.com/docs/user/en/guides/app-development/insert-a-document-via-api"/>
+    <hyperlink ref="A29" r:id="rId25" display="https://frappeframework.com/docs/user/en/guides/app-development/overriding-link-query-by-custom-script"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -3603,10 +3650,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3617,22 +3664,37 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>346</v>
+        <v>356</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>347</v>
+        <v>357</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>348</v>
+        <v>358</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>349</v>
+        <v>359</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>362</v>
       </c>
     </row>
   </sheetData>
@@ -3664,36 +3726,36 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" s="63" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="63" t="s">
-        <v>350</v>
-      </c>
-      <c r="B1" s="64" t="s">
-        <v>351</v>
+    <row r="1" s="64" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="64" t="s">
+        <v>363</v>
+      </c>
+      <c r="B1" s="65" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>352</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>353</v>
+        <v>365</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>354</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="5" s="66" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="65" t="s">
-        <v>356</v>
-      </c>
-      <c r="B5" s="65" t="s">
-        <v>357</v>
+        <v>367</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="5" s="67" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="66" t="s">
+        <v>369</v>
+      </c>
+      <c r="B5" s="66" t="s">
+        <v>370</v>
       </c>
     </row>
   </sheetData>
@@ -3716,15 +3778,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="72.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="86.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="79.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="49.42"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.52"/>
@@ -3732,29 +3794,38 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>186</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>187</v>
+        <v>188</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>358</v>
+        <v>371</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>359</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>360</v>
+        <v>372</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="10" t="s">
+        <v>374</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>375</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1" display="https://frappeframework.com/docs/user/en/guides/app-development/exporting-customizations"/>
     <hyperlink ref="B4" r:id="rId2" display="https://frappeframework.com/docs/user/en/guides/app-development/how-to-create-custom-fields-during-app-installation"/>
+    <hyperlink ref="B5" r:id="rId3" display="https://frappe.io/frappejs/docs/models/document.md"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
@@ -3771,10 +3842,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A17"/>
+  <dimension ref="A1:A20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
+      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3854,7 +3925,20 @@
         <v>18</v>
       </c>
     </row>
+    <row r="19" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A20" r:id="rId1" display="https://frappebooks.com/docs"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -3884,12 +3968,12 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
-        <v>20</v>
+      <c r="A3" s="8" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -3921,293 +4005,293 @@
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
-        <v>21</v>
+      <c r="A2" s="9" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
-        <v>22</v>
+      <c r="A3" s="10" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="s">
-        <v>23</v>
+      <c r="A4" s="10" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9" t="s">
-        <v>24</v>
+      <c r="A5" s="11" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8" t="s">
-        <v>26</v>
+      <c r="A9" s="10" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8" t="s">
-        <v>27</v>
+      <c r="A10" s="10" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="8" t="s">
-        <v>28</v>
+      <c r="A11" s="10" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="8" t="s">
-        <v>29</v>
+      <c r="A12" s="10" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="8" t="s">
-        <v>34</v>
+      <c r="A18" s="10" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="10" t="s">
-        <v>36</v>
+      <c r="A20" s="12" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="11" t="s">
-        <v>38</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="13" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="8" t="s">
-        <v>39</v>
+      <c r="A25" s="10" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="27" s="13" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="13" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="29" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="14" t="s">
         <v>42</v>
       </c>
     </row>
+    <row r="27" s="15" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" s="17" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="16" t="s">
+        <v>44</v>
+      </c>
+    </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="10" t="s">
-        <v>43</v>
+      <c r="A30" s="12" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="16" t="s">
-        <v>44</v>
+      <c r="A31" s="7" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="16" t="s">
-        <v>45</v>
+      <c r="A32" s="7" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="17" t="s">
-        <v>46</v>
+      <c r="A33" s="18" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="16" t="s">
-        <v>47</v>
+      <c r="A34" s="7" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="16" t="s">
-        <v>48</v>
+      <c r="A35" s="7" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="9" t="s">
-        <v>50</v>
+      <c r="A37" s="11" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="40" s="19" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="18" t="s">
-        <v>52</v>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="40" s="20" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="19" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="8" t="s">
-        <v>53</v>
+      <c r="A41" s="10" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="45" s="21" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="20" t="s">
-        <v>56</v>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="45" s="22" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="21" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="47" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="22" t="s">
-        <v>58</v>
+      <c r="A46" s="9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="47" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="23" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="7" t="s">
-        <v>59</v>
+      <c r="A48" s="9" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="7" t="s">
-        <v>60</v>
+      <c r="A49" s="9" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="7" t="s">
-        <v>61</v>
+      <c r="A50" s="9" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="7" t="s">
-        <v>62</v>
+      <c r="A51" s="9" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="7" t="s">
-        <v>63</v>
+      <c r="A52" s="9" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="7" t="s">
-        <v>64</v>
+      <c r="A53" s="9" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="7" t="s">
-        <v>65</v>
+      <c r="A54" s="9" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="57" s="23" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="23" t="s">
-        <v>67</v>
+      <c r="A55" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="57" s="24" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="24" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="16" t="s">
-        <v>70</v>
+      <c r="A60" s="7" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="16" t="s">
-        <v>71</v>
+      <c r="A61" s="7" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="16" t="s">
-        <v>72</v>
+      <c r="A62" s="7" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="16" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="65" s="25" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="24" t="s">
-        <v>74</v>
+      <c r="A63" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="65" s="26" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="25" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="16" t="s">
-        <v>75</v>
+      <c r="A66" s="7" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="16" t="s">
-        <v>76</v>
+      <c r="A67" s="7" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="16" t="s">
-        <v>77</v>
+      <c r="A68" s="7" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="16" t="s">
-        <v>78</v>
+      <c r="A69" s="7" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -4229,9 +4313,9 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C74"/>
+  <dimension ref="A1:C75"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A47" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A72" activeCellId="0" sqref="A72"/>
     </sheetView>
   </sheetViews>
@@ -4245,463 +4329,471 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" s="27" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="26" t="s">
-        <v>81</v>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" s="28" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="27" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="s">
-        <v>82</v>
+      <c r="A4" s="10" t="s">
+        <v>84</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="5" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="B5" s="9" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="6" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9" t="s">
+    <row r="5" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B5" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="C6" s="9" t="s">
+    </row>
+    <row r="6" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="11" t="s">
         <v>88</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>90</v>
+        <v>91</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="9" t="s">
-        <v>91</v>
+      <c r="A8" s="11" t="s">
+        <v>93</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>94</v>
+      <c r="A9" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>96</v>
+      <c r="A10" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>98</v>
+      <c r="A11" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="9"/>
-    </row>
-    <row r="13" s="27" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="27" t="s">
-        <v>99</v>
+      <c r="A12" s="11"/>
+    </row>
+    <row r="13" s="28" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="28" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="15" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="B15" s="9" t="s">
         <v>103</v>
+      </c>
+    </row>
+    <row r="15" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>110</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="18" s="9" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>111</v>
+      </c>
+    </row>
+    <row r="18" s="11" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>112</v>
+        <v>113</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="23" s="29" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="28" t="s">
-        <v>117</v>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="23" s="30" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="29" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="17.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>119</v>
+      <c r="A24" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>123</v>
+        <v>124</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="17.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>125</v>
+      <c r="A27" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="17.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="B28" s="8" t="s">
+      <c r="A28" s="10" t="s">
         <v>126</v>
       </c>
+      <c r="B28" s="10" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="17.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>128</v>
+      <c r="A29" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="17.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>130</v>
+      <c r="A30" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>132</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="17.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>133</v>
+      <c r="A31" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="17.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="B32" s="10" t="s">
-        <v>135</v>
+      <c r="A32" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="17.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="8"/>
-      <c r="B33" s="8"/>
+      <c r="A33" s="10"/>
+      <c r="B33" s="10"/>
     </row>
     <row r="34" customFormat="false" ht="17.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="8"/>
-      <c r="B34" s="8"/>
+      <c r="A34" s="10"/>
+      <c r="B34" s="10"/>
     </row>
     <row r="35" customFormat="false" ht="17.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="8"/>
-      <c r="B35" s="8"/>
-    </row>
-    <row r="36" s="31" customFormat="true" ht="17.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="B36" s="30"/>
+      <c r="A35" s="10"/>
+      <c r="B35" s="10"/>
+    </row>
+    <row r="36" s="32" customFormat="true" ht="17.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="B36" s="31"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="B37" s="9" t="s">
-        <v>138</v>
+      <c r="A37" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="B38" s="9" t="s">
-        <v>140</v>
+      <c r="A38" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="B39" s="9" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="43" s="32" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="32" t="s">
+      <c r="A39" s="11" t="s">
         <v>143</v>
       </c>
+      <c r="B39" s="11" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="43" s="33" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="33" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="46" s="33" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="33" t="s">
+      <c r="A44" s="11" t="s">
         <v>146</v>
       </c>
+      <c r="B44" s="10" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="46" s="34" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="34" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="B47" s="9" t="s">
-        <v>148</v>
+      <c r="A47" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="B47" s="11" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="B48" s="16" t="s">
-        <v>150</v>
+      <c r="A48" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="9" t="s">
-        <v>151</v>
+      <c r="A49" s="11" t="s">
+        <v>153</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>157</v>
-      </c>
-      <c r="B52" s="16" t="s">
-        <v>158</v>
+        <v>159</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>159</v>
-      </c>
-      <c r="B53" s="16" t="s">
-        <v>160</v>
+        <v>161</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="B55" s="8" t="s">
-        <v>164</v>
+      <c r="A55" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="B55" s="10" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="58" s="34" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="34" t="s">
-        <v>167</v>
+        <v>168</v>
+      </c>
+    </row>
+    <row r="58" s="35" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="35" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="B59" s="16" t="s">
-        <v>169</v>
+      <c r="A59" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="B60" s="16" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="63" s="35" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="35" t="s">
         <v>172</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="63" s="36" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="36" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>173</v>
-      </c>
-      <c r="B64" s="8" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="66" s="36" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="36" t="s">
         <v>175</v>
+      </c>
+      <c r="B64" s="10" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="66" s="37" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="37" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>176</v>
-      </c>
-      <c r="B68" s="9" t="s">
-        <v>177</v>
+        <v>178</v>
+      </c>
+      <c r="B68" s="11" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>178</v>
-      </c>
-      <c r="B69" s="16" t="s">
-        <v>179</v>
+        <v>180</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>180</v>
-      </c>
-      <c r="B70" s="16" t="s">
-        <v>181</v>
+        <v>182</v>
+      </c>
+      <c r="B70" s="7" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>182</v>
-      </c>
-      <c r="B71" s="8" t="s">
-        <v>183</v>
+        <v>184</v>
+      </c>
+      <c r="B71" s="12" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="8" t="s">
-        <v>184</v>
+      <c r="A72" s="10" t="s">
+        <v>186</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>187</v>
+        <v>189</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="B75" s="12" t="s">
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -4715,7 +4807,8 @@
     <hyperlink ref="B60" r:id="rId7" display="https://frappeframework.com/docs/user/en/api/server-calls"/>
     <hyperlink ref="B69" r:id="rId8" display="https://frappe.github.io/charts/"/>
     <hyperlink ref="B70" r:id="rId9" display="https://frappeframework.com/docs/user/en/guides/desk/formatter_for_link_fields"/>
-    <hyperlink ref="B71" r:id="rId10" display="https://github.com/org/app_name"/>
+    <hyperlink ref="B71" r:id="rId10" display="bench get-app https://github.com/org/app_name + &#10;bench --site site_name install-app app_name"/>
+    <hyperlink ref="B75" r:id="rId11" display="https://frappeframework.com/docs/user/en/guides/app-development/insert-a-document-via-api"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -4745,63 +4838,63 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="9" t="s">
-        <v>19</v>
+      <c r="A1" s="11" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="s">
-        <v>188</v>
+      <c r="A2" s="10" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
-        <v>190</v>
+      <c r="A4" s="8" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9" t="s">
-        <v>191</v>
+      <c r="A6" s="11" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="91.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8" t="s">
-        <v>192</v>
+      <c r="A7" s="10" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8" t="s">
-        <v>193</v>
+      <c r="A9" s="10" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="9" t="s">
-        <v>198</v>
+      <c r="A15" s="11" t="s">
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -4832,159 +4925,159 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" s="38" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="37" t="s">
-        <v>117</v>
+    <row r="1" s="39" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="38" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="s">
-        <v>199</v>
+      <c r="A2" s="10" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="9" t="s">
-        <v>201</v>
+      <c r="A4" s="11" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="s">
-        <v>202</v>
+      <c r="A5" s="10" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="10" s="40" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="39" t="s">
-        <v>207</v>
+        <v>210</v>
+      </c>
+    </row>
+    <row r="10" s="41" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="40" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="8" t="s">
-        <v>210</v>
+      <c r="A13" s="10" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="8" t="s">
-        <v>211</v>
+      <c r="A14" s="10" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="16" t="s">
-        <v>214</v>
+      <c r="A17" s="7" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="16" t="s">
-        <v>215</v>
+      <c r="A18" s="7" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="16" t="s">
-        <v>216</v>
+      <c r="A19" s="7" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="16" t="s">
-        <v>217</v>
+      <c r="A20" s="7" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="10" t="s">
-        <v>218</v>
+      <c r="A21" s="12" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="8" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="24" s="42" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="41" t="s">
-        <v>143</v>
+      <c r="A23" s="10" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="24" s="43" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="42" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="16" t="s">
-        <v>225</v>
+      <c r="A29" s="7" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="16" t="s">
-        <v>226</v>
+      <c r="A30" s="7" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
     </row>
   </sheetData>
@@ -5016,234 +5109,234 @@
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="s">
-        <v>228</v>
+      <c r="A2" s="10" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
-        <v>229</v>
+      <c r="A3" s="10" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="s">
-        <v>230</v>
+      <c r="A4" s="10" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="s">
-        <v>231</v>
+      <c r="A5" s="10" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8" t="s">
-        <v>232</v>
+      <c r="A6" s="10" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8" t="s">
-        <v>233</v>
+      <c r="A7" s="10" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="11" s="44" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="43" t="s">
-        <v>236</v>
+        <v>239</v>
+      </c>
+    </row>
+    <row r="11" s="45" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="44" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="8" t="s">
-        <v>237</v>
+      <c r="A13" s="10" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="8" t="s">
-        <v>238</v>
+      <c r="A14" s="10" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="8" t="s">
-        <v>239</v>
+      <c r="A15" s="10" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="9" t="s">
-        <v>241</v>
+      <c r="A17" s="11" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="21" s="45" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="45" t="s">
-        <v>244</v>
+        <v>247</v>
+      </c>
+    </row>
+    <row r="21" s="46" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="46" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="8" t="s">
-        <v>245</v>
+      <c r="A23" s="10" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="16" t="s">
-        <v>246</v>
+      <c r="A24" s="7" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="16" t="s">
-        <v>248</v>
+      <c r="A26" s="7" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="16" t="s">
-        <v>250</v>
+      <c r="A28" s="7" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="32" s="46" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="46" t="s">
-        <v>254</v>
+        <v>257</v>
+      </c>
+    </row>
+    <row r="32" s="47" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="47" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="47" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="39" s="46" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="46" t="s">
-        <v>260</v>
+      <c r="A37" s="48" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="39" s="47" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="47" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="16" t="s">
-        <v>261</v>
+      <c r="A40" s="7" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="16" t="s">
-        <v>262</v>
+      <c r="A41" s="7" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="46" s="36" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>269</v>
+      </c>
+    </row>
+    <row r="46" s="37" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="16" t="s">
-        <v>267</v>
+      <c r="A49" s="7" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="16" t="s">
-        <v>268</v>
+      <c r="A50" s="7" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="47" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="53" s="46" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="46" t="s">
-        <v>270</v>
+      <c r="A51" s="48" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="53" s="47" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="47" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="8" t="s">
-        <v>271</v>
+      <c r="A54" s="10" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="16" t="s">
-        <v>272</v>
+      <c r="A55" s="7" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="10" t="s">
-        <v>273</v>
+      <c r="A56" s="12" t="s">
+        <v>277</v>
       </c>
     </row>
   </sheetData>
@@ -5265,7 +5358,7 @@
   <dimension ref="A2:A27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5274,112 +5367,112 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="2" s="49" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="48" t="s">
-        <v>274</v>
+    <row r="2" s="50" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="49" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="16" t="s">
-        <v>276</v>
+      <c r="A4" s="7" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="s">
-        <v>277</v>
+      <c r="A5" s="10" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="16" t="s">
-        <v>279</v>
+      <c r="A7" s="7" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="11" s="51" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="50" t="s">
-        <v>282</v>
+        <v>285</v>
+      </c>
+    </row>
+    <row r="11" s="52" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="51" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="16" s="53" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="52" t="s">
-        <v>286</v>
+        <v>289</v>
+      </c>
+    </row>
+    <row r="16" s="54" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="53" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="19" s="55" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="54" t="s">
-        <v>288</v>
+        <v>291</v>
+      </c>
+    </row>
+    <row r="19" s="56" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="55" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="8" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="22" s="57" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="56" t="s">
-        <v>290</v>
+      <c r="A20" s="10" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="22" s="58" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="57" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="8" t="s">
-        <v>291</v>
+      <c r="A23" s="10" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="8" t="s">
-        <v>292</v>
+      <c r="A24" s="10" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="8" t="s">
-        <v>293</v>
+      <c r="A25" s="10" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="8"/>
-    </row>
-    <row r="27" s="59" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="58" t="s">
-        <v>294</v>
+      <c r="A26" s="10"/>
+    </row>
+    <row r="27" s="60" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="59" t="s">
+        <v>298</v>
       </c>
     </row>
   </sheetData>

</xml_diff>